<commit_message>
add check data date - filtering data
</commit_message>
<xml_diff>
--- a/stocksDB_edit.xlsx
+++ b/stocksDB_edit.xlsx
@@ -503,13 +503,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D826"/>
+  <dimension ref="A1:E826"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A799" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="10.6" customWidth="1" style="5" min="1" max="1025"/>
   </cols>
@@ -530,6 +530,14 @@
           <t>상장주식수</t>
         </is>
       </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>2962377</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="n">
+        <v>4.64</v>
+      </c>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="6">
       <c r="A2" s="8" t="inlineStr">
@@ -550,6 +558,9 @@
           <t>3615</t>
         </is>
       </c>
+      <c r="E2" s="5" t="n">
+        <v>7.916666666666667</v>
+      </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="6">
       <c r="A3" s="8" t="inlineStr">
@@ -570,6 +581,9 @@
           <t>5996</t>
         </is>
       </c>
+      <c r="E3" s="5" t="n">
+        <v>-5.766666666666667</v>
+      </c>
     </row>
     <row r="4" ht="12.8" customHeight="1" s="6">
       <c r="A4" s="8" t="inlineStr">
@@ -590,6 +604,9 @@
           <t>8093</t>
         </is>
       </c>
+      <c r="E4" s="5" t="n">
+        <v>6.536666666666666</v>
+      </c>
     </row>
     <row r="5" ht="12.8" customHeight="1" s="6">
       <c r="A5" s="8" t="inlineStr">
@@ -610,6 +627,9 @@
           <t>15689</t>
         </is>
       </c>
+      <c r="E5" s="5" t="n">
+        <v>1.42</v>
+      </c>
     </row>
     <row r="6" ht="12.8" customHeight="1" s="6">
       <c r="A6" s="8" t="inlineStr">
@@ -630,6 +650,9 @@
           <t>93257</t>
         </is>
       </c>
+      <c r="E6" s="5" t="n">
+        <v>2.92</v>
+      </c>
     </row>
     <row r="7" ht="12.8" customHeight="1" s="6">
       <c r="A7" s="8" t="inlineStr">
@@ -650,6 +673,9 @@
           <t>4818</t>
         </is>
       </c>
+      <c r="E7" s="5" t="n">
+        <v>2.13</v>
+      </c>
     </row>
     <row r="8" ht="12.8" customHeight="1" s="6">
       <c r="A8" s="8" t="inlineStr">
@@ -670,6 +696,9 @@
           <t>50660</t>
         </is>
       </c>
+      <c r="E8" s="5" t="n">
+        <v>1.886666666666667</v>
+      </c>
     </row>
     <row r="9" ht="12.8" customHeight="1" s="6">
       <c r="A9" s="8" t="inlineStr">
@@ -690,6 +719,9 @@
           <t>671</t>
         </is>
       </c>
+      <c r="E9" s="5" t="n">
+        <v>1.106666666666667</v>
+      </c>
     </row>
     <row r="10" ht="12.8" customHeight="1" s="6">
       <c r="A10" s="8" t="inlineStr">
@@ -710,6 +742,9 @@
           <t>2569</t>
         </is>
       </c>
+      <c r="E10" s="5" t="n">
+        <v>1.956666666666667</v>
+      </c>
     </row>
     <row r="11" ht="12.8" customHeight="1" s="6">
       <c r="A11" s="8" t="inlineStr">
@@ -730,6 +765,9 @@
           <t>4378</t>
         </is>
       </c>
+      <c r="E11" s="5" t="n">
+        <v>1.926666666666667</v>
+      </c>
     </row>
     <row r="12" ht="12.8" customHeight="1" s="6">
       <c r="A12" s="8" t="inlineStr">
@@ -750,6 +788,9 @@
           <t>9170</t>
         </is>
       </c>
+      <c r="E12" s="5" t="n">
+        <v>4.553333333333334</v>
+      </c>
     </row>
     <row r="13" ht="12.8" customHeight="1" s="6">
       <c r="A13" s="8" t="inlineStr">
@@ -770,6 +811,9 @@
           <t>66411</t>
         </is>
       </c>
+      <c r="E13" s="5" t="n">
+        <v>4.443333333333333</v>
+      </c>
     </row>
     <row r="14" ht="12.8" customHeight="1" s="6">
       <c r="A14" s="8" t="inlineStr">
@@ -790,6 +834,9 @@
           <t>11061</t>
         </is>
       </c>
+      <c r="E14" s="5" t="n">
+        <v>11.11666666666667</v>
+      </c>
     </row>
     <row r="15" ht="12.8" customHeight="1" s="6">
       <c r="A15" s="8" t="inlineStr">
@@ -810,6 +857,9 @@
           <t>54984</t>
         </is>
       </c>
+      <c r="E15" s="5" t="n">
+        <v>3.21</v>
+      </c>
     </row>
     <row r="16" ht="12.8" customHeight="1" s="6">
       <c r="A16" s="8" t="inlineStr">
@@ -830,6 +880,9 @@
           <t>5507</t>
         </is>
       </c>
+      <c r="E16" s="5" t="n">
+        <v>2.67</v>
+      </c>
     </row>
     <row r="17" ht="12.8" customHeight="1" s="6">
       <c r="A17" s="8" t="inlineStr">
@@ -850,6 +903,9 @@
           <t>9579</t>
         </is>
       </c>
+      <c r="E17" s="5" t="n">
+        <v>6.649999999999999</v>
+      </c>
     </row>
     <row r="18" ht="12.8" customHeight="1" s="6">
       <c r="A18" s="8" t="inlineStr">
@@ -870,6 +926,9 @@
           <t>39332</t>
         </is>
       </c>
+      <c r="E18" s="5" t="n">
+        <v>8.84</v>
+      </c>
     </row>
     <row r="19" ht="12.8" customHeight="1" s="6">
       <c r="A19" s="8" t="inlineStr">
@@ -890,6 +949,9 @@
           <t>41679</t>
         </is>
       </c>
+      <c r="E19" s="5" t="n">
+        <v/>
+      </c>
     </row>
     <row r="20" ht="12.8" customHeight="1" s="6">
       <c r="A20" s="8" t="inlineStr">
@@ -910,6 +972,9 @@
           <t>1759</t>
         </is>
       </c>
+      <c r="E20" s="5" t="n">
+        <v>2.43</v>
+      </c>
     </row>
     <row r="21" ht="12.8" customHeight="1" s="6">
       <c r="A21" s="8" t="inlineStr">
@@ -930,6 +995,9 @@
           <t>1538</t>
         </is>
       </c>
+      <c r="E21" s="5" t="n">
+        <v>1.693333333333333</v>
+      </c>
     </row>
     <row r="22" ht="12.8" customHeight="1" s="6">
       <c r="A22" s="8" t="inlineStr">
@@ -950,6 +1018,9 @@
           <t>13079</t>
         </is>
       </c>
+      <c r="E22" s="5" t="n">
+        <v>3.523333333333333</v>
+      </c>
     </row>
     <row r="23" ht="12.8" customHeight="1" s="6">
       <c r="A23" s="8" t="inlineStr">
@@ -970,6 +1041,9 @@
           <t>11264</t>
         </is>
       </c>
+      <c r="E23" s="5" t="n">
+        <v>0.88</v>
+      </c>
     </row>
     <row r="24" ht="12.8" customHeight="1" s="6">
       <c r="A24" s="8" t="inlineStr">
@@ -990,6 +1064,9 @@
           <t>5474</t>
         </is>
       </c>
+      <c r="E24" s="5" t="n">
+        <v/>
+      </c>
     </row>
     <row r="25" ht="12.8" customHeight="1" s="6">
       <c r="A25" s="8" t="inlineStr">
@@ -1010,6 +1087,9 @@
           <t>19338</t>
         </is>
       </c>
+      <c r="E25" s="5" t="n">
+        <v>51.29333333333333</v>
+      </c>
     </row>
     <row r="26" ht="12.8" customHeight="1" s="6">
       <c r="A26" s="8" t="inlineStr">
@@ -1030,6 +1110,9 @@
           <t>46253</t>
         </is>
       </c>
+      <c r="E26" s="5" t="n">
+        <v>3.106666666666667</v>
+      </c>
     </row>
     <row r="27" ht="12.8" customHeight="1" s="6">
       <c r="A27" s="8" t="inlineStr">
@@ -1050,6 +1133,9 @@
           <t>102886</t>
         </is>
       </c>
+      <c r="E27" s="5" t="n">
+        <v>5.183333333333334</v>
+      </c>
     </row>
     <row r="28" ht="12.8" customHeight="1" s="6">
       <c r="A28" s="8" t="inlineStr">
@@ -1070,6 +1156,9 @@
           <t>23876</t>
         </is>
       </c>
+      <c r="E28" s="5" t="n">
+        <v>1.633333333333334</v>
+      </c>
     </row>
     <row r="29" ht="12.8" customHeight="1" s="6">
       <c r="A29" s="8" t="inlineStr">
@@ -1090,6 +1179,9 @@
           <t>28774</t>
         </is>
       </c>
+      <c r="E29" s="5" t="n">
+        <v>2.093333333333333</v>
+      </c>
     </row>
     <row r="30" ht="12.8" customHeight="1" s="6">
       <c r="A30" s="8" t="inlineStr">
@@ -1110,6 +1202,9 @@
           <t>4321</t>
         </is>
       </c>
+      <c r="E30" s="5" t="n">
+        <v>-12.39333333333333</v>
+      </c>
     </row>
     <row r="31" ht="12.8" customHeight="1" s="6">
       <c r="A31" s="8" t="inlineStr">
@@ -1130,6 +1225,9 @@
           <t>4165</t>
         </is>
       </c>
+      <c r="E31" s="5" t="n">
+        <v>8.366666666666667</v>
+      </c>
     </row>
     <row r="32" ht="12.8" customHeight="1" s="6">
       <c r="A32" s="8" t="inlineStr">
@@ -1150,6 +1248,9 @@
           <t>19545</t>
         </is>
       </c>
+      <c r="E32" s="5" t="n">
+        <v>3.103333333333333</v>
+      </c>
     </row>
     <row r="33" ht="12.8" customHeight="1" s="6">
       <c r="A33" s="8" t="inlineStr">
@@ -1170,6 +1271,9 @@
           <t>10124</t>
         </is>
       </c>
+      <c r="E33" s="5" t="n">
+        <v>3.73</v>
+      </c>
     </row>
     <row r="34" ht="12.8" customHeight="1" s="6">
       <c r="A34" s="8" t="inlineStr">
@@ -1190,6 +1294,9 @@
           <t>1149</t>
         </is>
       </c>
+      <c r="E34" s="5" t="n">
+        <v>-2.9</v>
+      </c>
     </row>
     <row r="35" ht="12.8" customHeight="1" s="6">
       <c r="A35" s="8" t="inlineStr">
@@ -1210,6 +1317,9 @@
           <t>41574</t>
         </is>
       </c>
+      <c r="E35" s="5" t="n">
+        <v>4.266666666666667</v>
+      </c>
     </row>
     <row r="36" ht="12.8" customHeight="1" s="6">
       <c r="A36" s="8" t="inlineStr">
@@ -1230,6 +1340,9 @@
           <t>1315</t>
         </is>
       </c>
+      <c r="E36" s="5" t="n">
+        <v>3.26</v>
+      </c>
     </row>
     <row r="37" ht="12.8" customHeight="1" s="6">
       <c r="A37" s="8" t="inlineStr">
@@ -1250,6 +1363,9 @@
           <t>2012</t>
         </is>
       </c>
+      <c r="E37" s="5" t="n">
+        <v>-0.1566666666666666</v>
+      </c>
     </row>
     <row r="38" ht="12.8" customHeight="1" s="6">
       <c r="A38" s="8" t="inlineStr">
@@ -1270,6 +1386,9 @@
           <t>932</t>
         </is>
       </c>
+      <c r="E38" s="5" t="n">
+        <v>-0.9133333333333334</v>
+      </c>
     </row>
     <row r="39" ht="12.8" customHeight="1" s="6">
       <c r="A39" s="8" t="inlineStr">
@@ -1290,6 +1409,9 @@
           <t>474606</t>
         </is>
       </c>
+      <c r="E39" s="5" t="n">
+        <v>3.266666666666667</v>
+      </c>
     </row>
     <row r="40" ht="12.8" customHeight="1" s="6">
       <c r="A40" s="8" t="inlineStr">
@@ -1306,6 +1428,9 @@
         <v>101414285</v>
       </c>
       <c r="D40" s="5" t="n"/>
+      <c r="E40" s="5" t="n">
+        <v/>
+      </c>
     </row>
     <row r="41" ht="12.8" customHeight="1" s="6">
       <c r="A41" s="8" t="inlineStr">
@@ -1326,6 +1451,9 @@
           <t>2222</t>
         </is>
       </c>
+      <c r="E41" s="5" t="n">
+        <v>3.186666666666667</v>
+      </c>
     </row>
     <row r="42" ht="12.8" customHeight="1" s="6">
       <c r="A42" s="8" t="inlineStr">
@@ -1346,6 +1474,9 @@
           <t>11504</t>
         </is>
       </c>
+      <c r="E42" s="5" t="n">
+        <v>5.996666666666666</v>
+      </c>
     </row>
     <row r="43" ht="12.8" customHeight="1" s="6">
       <c r="A43" s="8" t="inlineStr">
@@ -1366,6 +1497,9 @@
           <t>4738</t>
         </is>
       </c>
+      <c r="E43" s="5" t="n">
+        <v>5.793333333333333</v>
+      </c>
     </row>
     <row r="44" ht="12.8" customHeight="1" s="6">
       <c r="A44" s="8" t="inlineStr">
@@ -1386,6 +1520,9 @@
           <t>4222</t>
         </is>
       </c>
+      <c r="E44" s="5" t="n">
+        <v>-0.08333333333333333</v>
+      </c>
     </row>
     <row r="45" ht="12.8" customHeight="1" s="6">
       <c r="A45" s="8" t="inlineStr">
@@ -1406,6 +1543,9 @@
           <t>9485</t>
         </is>
       </c>
+      <c r="E45" s="5" t="n">
+        <v>4.23</v>
+      </c>
     </row>
     <row r="46" ht="12.8" customHeight="1" s="6">
       <c r="A46" s="8" t="inlineStr">
@@ -1426,6 +1566,9 @@
           <t>5664</t>
         </is>
       </c>
+      <c r="E46" s="5" t="n">
+        <v>2.943333333333333</v>
+      </c>
     </row>
     <row r="47" ht="12.8" customHeight="1" s="6">
       <c r="A47" s="8" t="inlineStr">
@@ -1446,6 +1589,9 @@
           <t>8212</t>
         </is>
       </c>
+      <c r="E47" s="5" t="n">
+        <v>1.93</v>
+      </c>
     </row>
     <row r="48" ht="12.8" customHeight="1" s="6">
       <c r="A48" s="8" t="inlineStr">
@@ -1466,6 +1612,9 @@
           <t>370</t>
         </is>
       </c>
+      <c r="E48" s="5" t="n">
+        <v>-8.606666666666667</v>
+      </c>
     </row>
     <row r="49" ht="12.8" customHeight="1" s="6">
       <c r="A49" s="8" t="inlineStr">
@@ -1486,6 +1635,9 @@
           <t>13349</t>
         </is>
       </c>
+      <c r="E49" s="5" t="n">
+        <v>3.08</v>
+      </c>
     </row>
     <row r="50" ht="12.8" customHeight="1" s="6">
       <c r="A50" s="8" t="inlineStr">
@@ -1506,6 +1658,9 @@
           <t>131189</t>
         </is>
       </c>
+      <c r="E50" s="5" t="n">
+        <v>3.226666666666667</v>
+      </c>
     </row>
     <row r="51" ht="12.8" customHeight="1" s="6">
       <c r="A51" s="8" t="inlineStr">
@@ -1526,6 +1681,9 @@
           <t>212465</t>
         </is>
       </c>
+      <c r="E51" s="5" t="n">
+        <v>4.12</v>
+      </c>
     </row>
     <row r="52" ht="12.8" customHeight="1" s="6">
       <c r="A52" s="8" t="inlineStr">
@@ -1546,6 +1704,9 @@
           <t>53880</t>
         </is>
       </c>
+      <c r="E52" s="5" t="n">
+        <v>5.55</v>
+      </c>
     </row>
     <row r="53" ht="12.8" customHeight="1" s="6">
       <c r="A53" s="8" t="inlineStr">
@@ -1566,6 +1727,9 @@
           <t>79661</t>
         </is>
       </c>
+      <c r="E53" s="5" t="n">
+        <v>3.56</v>
+      </c>
     </row>
     <row r="54" ht="12.8" customHeight="1" s="6">
       <c r="A54" s="8" t="inlineStr">
@@ -1586,6 +1750,9 @@
           <t>76731</t>
         </is>
       </c>
+      <c r="E54" s="5" t="n">
+        <v>3.156666666666667</v>
+      </c>
     </row>
     <row r="55" ht="12.8" customHeight="1" s="6">
       <c r="A55" s="8" t="inlineStr">
@@ -1606,6 +1773,9 @@
           <t>33142</t>
         </is>
       </c>
+      <c r="E55" s="5" t="n">
+        <v>10.31333333333333</v>
+      </c>
     </row>
     <row r="56" ht="12.8" customHeight="1" s="6">
       <c r="A56" s="8" t="inlineStr">
@@ -1626,6 +1796,9 @@
           <t>172306</t>
         </is>
       </c>
+      <c r="E56" s="5" t="n">
+        <v>2.106666666666667</v>
+      </c>
     </row>
     <row r="57" ht="12.8" customHeight="1" s="6">
       <c r="A57" s="8" t="inlineStr">
@@ -1646,6 +1819,9 @@
           <t>216938</t>
         </is>
       </c>
+      <c r="E57" s="5" t="n">
+        <v>6.156666666666666</v>
+      </c>
     </row>
     <row r="58" ht="12.8" customHeight="1" s="6">
       <c r="A58" s="8" t="inlineStr">
@@ -1666,6 +1842,9 @@
           <t>7633</t>
         </is>
       </c>
+      <c r="E58" s="5" t="n">
+        <v>4.876666666666667</v>
+      </c>
     </row>
     <row r="59" ht="12.8" customHeight="1" s="6">
       <c r="A59" s="8" t="inlineStr">
@@ -1686,6 +1865,9 @@
           <t>14816</t>
         </is>
       </c>
+      <c r="E59" s="5" t="n">
+        <v>1.953333333333333</v>
+      </c>
     </row>
     <row r="60" ht="12.8" customHeight="1" s="6">
       <c r="A60" s="8" t="inlineStr">
@@ -1706,6 +1888,9 @@
           <t>5536</t>
         </is>
       </c>
+      <c r="E60" s="5" t="n">
+        <v>3.826666666666667</v>
+      </c>
     </row>
     <row r="61" ht="12.8" customHeight="1" s="6">
       <c r="A61" s="8" t="inlineStr">
@@ -1726,6 +1911,9 @@
           <t>35466</t>
         </is>
       </c>
+      <c r="E61" s="5" t="n">
+        <v>2.716666666666667</v>
+      </c>
     </row>
     <row r="62" ht="12.8" customHeight="1" s="6">
       <c r="A62" s="8" t="inlineStr">
@@ -1746,6 +1934,9 @@
           <t>8003</t>
         </is>
       </c>
+      <c r="E62" s="5" t="n">
+        <v>14.83</v>
+      </c>
     </row>
     <row r="63" ht="12.8" customHeight="1" s="6">
       <c r="A63" s="8" t="inlineStr">
@@ -1766,6 +1957,9 @@
           <t>17750</t>
         </is>
       </c>
+      <c r="E63" s="5" t="n">
+        <v>7.496666666666666</v>
+      </c>
     </row>
     <row r="64" ht="12.8" customHeight="1" s="6">
       <c r="A64" s="8" t="inlineStr">
@@ -1786,6 +1980,9 @@
           <t>628</t>
         </is>
       </c>
+      <c r="E64" s="5" t="n">
+        <v>3.173333333333333</v>
+      </c>
     </row>
     <row r="65" ht="12.8" customHeight="1" s="6">
       <c r="A65" s="8" t="inlineStr">
@@ -1806,6 +2003,9 @@
           <t>235356</t>
         </is>
       </c>
+      <c r="E65" s="5" t="n">
+        <v>35.57333333333333</v>
+      </c>
     </row>
     <row r="66" ht="12.8" customHeight="1" s="6">
       <c r="A66" s="8" t="inlineStr">
@@ -1826,6 +2026,9 @@
           <t>18343</t>
         </is>
       </c>
+      <c r="E66" s="5" t="n">
+        <v>2.27</v>
+      </c>
     </row>
     <row r="67" ht="12.8" customHeight="1" s="6">
       <c r="A67" s="8" t="inlineStr">
@@ -1842,6 +2045,9 @@
         <v>18660000</v>
       </c>
       <c r="D67" s="5" t="n"/>
+      <c r="E67" s="5" t="n">
+        <v/>
+      </c>
     </row>
     <row r="68" ht="12.8" customHeight="1" s="6">
       <c r="A68" s="8" t="inlineStr">
@@ -1862,6 +2068,9 @@
           <t>7469</t>
         </is>
       </c>
+      <c r="E68" s="5" t="n">
+        <v>2.67</v>
+      </c>
     </row>
     <row r="69" ht="12.8" customHeight="1" s="6">
       <c r="A69" s="8" t="inlineStr">
@@ -1882,6 +2091,9 @@
           <t>1419</t>
         </is>
       </c>
+      <c r="E69" s="5" t="n">
+        <v>5.583333333333333</v>
+      </c>
     </row>
     <row r="70" ht="12.8" customHeight="1" s="6">
       <c r="A70" s="8" t="inlineStr">
@@ -1902,6 +2114,9 @@
           <t>3223</t>
         </is>
       </c>
+      <c r="E70" s="5" t="n">
+        <v>2.83</v>
+      </c>
     </row>
     <row r="71" ht="12.8" customHeight="1" s="6">
       <c r="A71" s="8" t="inlineStr">
@@ -1922,6 +2137,9 @@
           <t>30714</t>
         </is>
       </c>
+      <c r="E71" s="5" t="n">
+        <v>7.976666666666667</v>
+      </c>
     </row>
     <row r="72" ht="12.8" customHeight="1" s="6">
       <c r="A72" s="8" t="inlineStr">
@@ -1942,6 +2160,9 @@
           <t>69880</t>
         </is>
       </c>
+      <c r="E72" s="5" t="n">
+        <v>7.253333333333334</v>
+      </c>
     </row>
     <row r="73" ht="12.8" customHeight="1" s="6">
       <c r="A73" s="8" t="inlineStr">
@@ -1962,6 +2183,9 @@
           <t>5998</t>
         </is>
       </c>
+      <c r="E73" s="5" t="n">
+        <v>3.406666666666667</v>
+      </c>
     </row>
     <row r="74" ht="12.8" customHeight="1" s="6">
       <c r="A74" s="8" t="inlineStr">
@@ -1982,6 +2206,9 @@
           <t>1230</t>
         </is>
       </c>
+      <c r="E74" s="5" t="n">
+        <v>-1.483333333333333</v>
+      </c>
     </row>
     <row r="75" ht="12.8" customHeight="1" s="6">
       <c r="A75" s="8" t="inlineStr">
@@ -2002,6 +2229,9 @@
           <t>406</t>
         </is>
       </c>
+      <c r="E75" s="5" t="n">
+        <v>5.133333333333334</v>
+      </c>
     </row>
     <row r="76" ht="12.8" customHeight="1" s="6">
       <c r="A76" s="8" t="inlineStr">
@@ -2022,6 +2252,9 @@
           <t>916</t>
         </is>
       </c>
+      <c r="E76" s="5" t="n">
+        <v>0.23</v>
+      </c>
     </row>
     <row r="77" ht="12.8" customHeight="1" s="6">
       <c r="A77" s="8" t="inlineStr">
@@ -2042,6 +2275,9 @@
           <t>5467</t>
         </is>
       </c>
+      <c r="E77" s="5" t="n">
+        <v>5.993333333333333</v>
+      </c>
     </row>
     <row r="78" ht="12.8" customHeight="1" s="6">
       <c r="A78" s="8" t="inlineStr">
@@ -2062,6 +2298,9 @@
           <t>1775</t>
         </is>
       </c>
+      <c r="E78" s="5" t="n">
+        <v>1.393333333333333</v>
+      </c>
     </row>
     <row r="79" ht="12.8" customHeight="1" s="6">
       <c r="A79" s="8" t="inlineStr">
@@ -2082,6 +2321,9 @@
           <t>1524</t>
         </is>
       </c>
+      <c r="E79" s="5" t="n">
+        <v>0.9466666666666667</v>
+      </c>
     </row>
     <row r="80" ht="12.8" customHeight="1" s="6">
       <c r="A80" s="8" t="inlineStr">
@@ -2102,6 +2344,9 @@
           <t>20012</t>
         </is>
       </c>
+      <c r="E80" s="5" t="n">
+        <v>3.866666666666667</v>
+      </c>
     </row>
     <row r="81" ht="12.8" customHeight="1" s="6">
       <c r="A81" s="8" t="inlineStr">
@@ -2122,6 +2367,9 @@
           <t>21174</t>
         </is>
       </c>
+      <c r="E81" s="5" t="n">
+        <v>4.136666666666667</v>
+      </c>
     </row>
     <row r="82" ht="12.8" customHeight="1" s="6">
       <c r="A82" s="8" t="inlineStr">
@@ -2142,6 +2390,9 @@
           <t>21985</t>
         </is>
       </c>
+      <c r="E82" s="5" t="n">
+        <v>1.546666666666667</v>
+      </c>
     </row>
     <row r="83" ht="12.8" customHeight="1" s="6">
       <c r="A83" s="8" t="inlineStr">
@@ -2162,6 +2413,9 @@
           <t>6393</t>
         </is>
       </c>
+      <c r="E83" s="5" t="n">
+        <v>7.636666666666667</v>
+      </c>
     </row>
     <row r="84" ht="12.8" customHeight="1" s="6">
       <c r="A84" s="8" t="inlineStr">
@@ -2182,6 +2436,9 @@
           <t>7766</t>
         </is>
       </c>
+      <c r="E84" s="5" t="n">
+        <v>1.506666666666667</v>
+      </c>
     </row>
     <row r="85" ht="12.8" customHeight="1" s="6">
       <c r="A85" s="8" t="inlineStr">
@@ -2202,6 +2459,9 @@
           <t>212483</t>
         </is>
       </c>
+      <c r="E85" s="5" t="n">
+        <v>3.396666666666667</v>
+      </c>
     </row>
     <row r="86" ht="12.8" customHeight="1" s="6">
       <c r="A86" s="8" t="inlineStr">
@@ -2222,6 +2482,9 @@
           <t>166604</t>
         </is>
       </c>
+      <c r="E86" s="5" t="n">
+        <v/>
+      </c>
     </row>
     <row r="87" ht="12.8" customHeight="1" s="6">
       <c r="A87" s="8" t="inlineStr">
@@ -2242,6 +2505,9 @@
           <t>22162</t>
         </is>
       </c>
+      <c r="E87" s="5" t="n">
+        <v>1.856666666666667</v>
+      </c>
     </row>
     <row r="88" ht="12.8" customHeight="1" s="6">
       <c r="A88" s="8" t="inlineStr">
@@ -2262,6 +2528,9 @@
           <t>173234</t>
         </is>
       </c>
+      <c r="E88" s="5" t="n">
+        <v>0.6366666666666666</v>
+      </c>
     </row>
     <row r="89" ht="12.8" customHeight="1" s="6">
       <c r="A89" s="8" t="inlineStr">
@@ -2282,6 +2551,9 @@
           <t>6079</t>
         </is>
       </c>
+      <c r="E89" s="5" t="n">
+        <v>2.256666666666666</v>
+      </c>
     </row>
     <row r="90" ht="12.8" customHeight="1" s="6">
       <c r="A90" s="8" t="inlineStr">
@@ -2302,6 +2574,9 @@
           <t>20535</t>
         </is>
       </c>
+      <c r="E90" s="5" t="n">
+        <v>3.73</v>
+      </c>
     </row>
     <row r="91" ht="12.8" customHeight="1" s="6">
       <c r="A91" s="8" t="inlineStr">
@@ -2322,6 +2597,9 @@
           <t>115793</t>
         </is>
       </c>
+      <c r="E91" s="5" t="n">
+        <v>4.543333333333334</v>
+      </c>
     </row>
     <row r="92" ht="12.8" customHeight="1" s="6">
       <c r="A92" s="8" t="inlineStr">
@@ -2342,6 +2620,9 @@
           <t>8576</t>
         </is>
       </c>
+      <c r="E92" s="5" t="n">
+        <v>3.3</v>
+      </c>
     </row>
     <row r="93" ht="12.8" customHeight="1" s="6">
       <c r="A93" s="8" t="inlineStr">
@@ -2362,6 +2643,9 @@
           <t>2448</t>
         </is>
       </c>
+      <c r="E93" s="5" t="n">
+        <v>1.733333333333333</v>
+      </c>
     </row>
     <row r="94" ht="12.8" customHeight="1" s="6">
       <c r="A94" s="8" t="inlineStr">
@@ -2382,6 +2666,9 @@
           <t>6529</t>
         </is>
       </c>
+      <c r="E94" s="5" t="n">
+        <v>3.146666666666667</v>
+      </c>
     </row>
     <row r="95" ht="12.8" customHeight="1" s="6">
       <c r="A95" s="8" t="inlineStr">
@@ -2402,6 +2689,9 @@
           <t>9501</t>
         </is>
       </c>
+      <c r="E95" s="5" t="n">
+        <v>2.853333333333333</v>
+      </c>
     </row>
     <row r="96" ht="12.8" customHeight="1" s="6">
       <c r="A96" s="8" t="inlineStr">
@@ -2422,6 +2712,9 @@
           <t>3350</t>
         </is>
       </c>
+      <c r="E96" s="5" t="n">
+        <v>4.226666666666667</v>
+      </c>
     </row>
     <row r="97" ht="12.8" customHeight="1" s="6">
       <c r="A97" s="8" t="inlineStr">
@@ -2442,6 +2735,9 @@
           <t>669</t>
         </is>
       </c>
+      <c r="E97" s="5" t="n">
+        <v>-9.626666666666667</v>
+      </c>
     </row>
     <row r="98" ht="12.8" customHeight="1" s="6">
       <c r="A98" s="8" t="inlineStr">
@@ -2462,6 +2758,9 @@
           <t>2840</t>
         </is>
       </c>
+      <c r="E98" s="5" t="n">
+        <v>0.1233333333333333</v>
+      </c>
     </row>
     <row r="99" ht="12.8" customHeight="1" s="6">
       <c r="A99" s="8" t="inlineStr">
@@ -2482,6 +2781,9 @@
           <t>1540</t>
         </is>
       </c>
+      <c r="E99" s="5" t="n">
+        <v>-1.593333333333333</v>
+      </c>
     </row>
     <row r="100" ht="12.8" customHeight="1" s="6">
       <c r="A100" s="8" t="inlineStr">
@@ -2502,6 +2804,9 @@
           <t>547</t>
         </is>
       </c>
+      <c r="E100" s="5" t="n">
+        <v>-9.85</v>
+      </c>
     </row>
     <row r="101" ht="12.8" customHeight="1" s="6">
       <c r="A101" s="8" t="inlineStr">
@@ -2522,6 +2827,9 @@
           <t>1509</t>
         </is>
       </c>
+      <c r="E101" s="5" t="n">
+        <v>7.163333333333333</v>
+      </c>
     </row>
     <row r="102" ht="12.8" customHeight="1" s="6">
       <c r="A102" s="8" t="inlineStr">
@@ -2542,6 +2850,9 @@
           <t>1201</t>
         </is>
       </c>
+      <c r="E102" s="5" t="n">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="103" ht="12.8" customHeight="1" s="6">
       <c r="A103" s="8" t="inlineStr">
@@ -2562,6 +2873,9 @@
           <t>2681</t>
         </is>
       </c>
+      <c r="E103" s="5" t="n">
+        <v>0.7333333333333334</v>
+      </c>
     </row>
     <row r="104" ht="12.8" customHeight="1" s="6">
       <c r="A104" s="8" t="inlineStr">
@@ -2582,6 +2896,9 @@
           <t>5907</t>
         </is>
       </c>
+      <c r="E104" s="5" t="n">
+        <v>2.65</v>
+      </c>
     </row>
     <row r="105" ht="12.8" customHeight="1" s="6">
       <c r="A105" s="8" t="inlineStr">
@@ -2602,6 +2919,9 @@
           <t>32528</t>
         </is>
       </c>
+      <c r="E105" s="5" t="n">
+        <v>-0.11</v>
+      </c>
     </row>
     <row r="106" ht="12.8" customHeight="1" s="6">
       <c r="A106" s="8" t="inlineStr">
@@ -2622,6 +2942,9 @@
           <t>331</t>
         </is>
       </c>
+      <c r="E106" s="5" t="n">
+        <v>4.563333333333333</v>
+      </c>
     </row>
     <row r="107" ht="12.8" customHeight="1" s="6">
       <c r="A107" s="8" t="inlineStr">
@@ -2642,6 +2965,9 @@
           <t>2124</t>
         </is>
       </c>
+      <c r="E107" s="5" t="n">
+        <v>2.616666666666667</v>
+      </c>
     </row>
     <row r="108" ht="12.8" customHeight="1" s="6">
       <c r="A108" s="8" t="inlineStr">
@@ -2662,6 +2988,9 @@
           <t>4504</t>
         </is>
       </c>
+      <c r="E108" s="5" t="n">
+        <v>6.733333333333333</v>
+      </c>
     </row>
     <row r="109" ht="12.8" customHeight="1" s="6">
       <c r="A109" s="8" t="inlineStr">
@@ -2682,6 +3011,9 @@
           <t>3751</t>
         </is>
       </c>
+      <c r="E109" s="5" t="n">
+        <v>2.016666666666667</v>
+      </c>
     </row>
     <row r="110" ht="12.8" customHeight="1" s="6">
       <c r="A110" s="8" t="inlineStr">
@@ -2702,6 +3034,9 @@
           <t>4317</t>
         </is>
       </c>
+      <c r="E110" s="5" t="n">
+        <v>1.143333333333333</v>
+      </c>
     </row>
     <row r="111" ht="12.8" customHeight="1" s="6">
       <c r="A111" s="8" t="inlineStr">
@@ -2722,6 +3057,9 @@
           <t>7522</t>
         </is>
       </c>
+      <c r="E111" s="5" t="n">
+        <v>0.9933333333333333</v>
+      </c>
     </row>
     <row r="112" ht="12.8" customHeight="1" s="6">
       <c r="A112" s="8" t="inlineStr">
@@ -2742,6 +3080,9 @@
           <t>1457</t>
         </is>
       </c>
+      <c r="E112" s="5" t="n">
+        <v>-1.656666666666667</v>
+      </c>
     </row>
     <row r="113" ht="12.8" customHeight="1" s="6">
       <c r="A113" s="8" t="inlineStr">
@@ -2762,6 +3103,9 @@
           <t>2303</t>
         </is>
       </c>
+      <c r="E113" s="5" t="n">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="114" ht="12.8" customHeight="1" s="6">
       <c r="A114" s="8" t="inlineStr">
@@ -2782,6 +3126,9 @@
           <t>596</t>
         </is>
       </c>
+      <c r="E114" s="5" t="n">
+        <v>2.17</v>
+      </c>
     </row>
     <row r="115" ht="12.8" customHeight="1" s="6">
       <c r="A115" s="8" t="inlineStr">
@@ -2802,6 +3149,9 @@
           <t>6990</t>
         </is>
       </c>
+      <c r="E115" s="5" t="n">
+        <v>8.299999999999999</v>
+      </c>
     </row>
     <row r="116" ht="12.8" customHeight="1" s="6">
       <c r="A116" s="8" t="inlineStr">
@@ -2822,6 +3172,9 @@
           <t>1832</t>
         </is>
       </c>
+      <c r="E116" s="5" t="n">
+        <v>-1.123333333333333</v>
+      </c>
     </row>
     <row r="117" ht="12.8" customHeight="1" s="6">
       <c r="A117" s="8" t="inlineStr">
@@ -2842,6 +3195,9 @@
           <t>1067</t>
         </is>
       </c>
+      <c r="E117" s="5" t="n">
+        <v>1.44</v>
+      </c>
     </row>
     <row r="118" ht="12.8" customHeight="1" s="6">
       <c r="A118" s="8" t="inlineStr">
@@ -2862,6 +3218,9 @@
           <t>76077</t>
         </is>
       </c>
+      <c r="E118" s="5" t="n">
+        <v>3.69</v>
+      </c>
     </row>
     <row r="119" ht="12.8" customHeight="1" s="6">
       <c r="A119" s="8" t="inlineStr">
@@ -2882,6 +3241,9 @@
           <t>15278</t>
         </is>
       </c>
+      <c r="E119" s="5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="120" ht="12.8" customHeight="1" s="6">
       <c r="A120" s="8" t="inlineStr">
@@ -2902,6 +3264,9 @@
           <t>4992</t>
         </is>
       </c>
+      <c r="E120" s="5" t="n">
+        <v>1.64</v>
+      </c>
     </row>
     <row r="121" ht="12.8" customHeight="1" s="6">
       <c r="A121" s="8" t="inlineStr">
@@ -2922,6 +3287,9 @@
           <t>1077</t>
         </is>
       </c>
+      <c r="E121" s="5" t="n">
+        <v>1.846666666666667</v>
+      </c>
     </row>
     <row r="122" ht="12.8" customHeight="1" s="6">
       <c r="A122" s="8" t="inlineStr">
@@ -2942,6 +3310,9 @@
           <t>2098</t>
         </is>
       </c>
+      <c r="E122" s="5" t="n">
+        <v>1.796666666666667</v>
+      </c>
     </row>
     <row r="123" ht="12.8" customHeight="1" s="6">
       <c r="A123" s="8" t="inlineStr">
@@ -2962,6 +3333,9 @@
           <t>7458</t>
         </is>
       </c>
+      <c r="E123" s="5" t="n">
+        <v>2.42</v>
+      </c>
     </row>
     <row r="124" ht="12.8" customHeight="1" s="6">
       <c r="A124" s="8" t="inlineStr">
@@ -2982,6 +3356,9 @@
           <t>13949</t>
         </is>
       </c>
+      <c r="E124" s="5" t="n">
+        <v>3.593333333333333</v>
+      </c>
     </row>
     <row r="125" ht="12.8" customHeight="1" s="6">
       <c r="A125" s="8" t="inlineStr">
@@ -3002,6 +3379,9 @@
           <t>1798</t>
         </is>
       </c>
+      <c r="E125" s="5" t="n">
+        <v>5.97</v>
+      </c>
     </row>
     <row r="126" ht="12.8" customHeight="1" s="6">
       <c r="A126" s="8" t="inlineStr">
@@ -3022,6 +3402,9 @@
           <t>8010</t>
         </is>
       </c>
+      <c r="E126" s="5" t="n">
+        <v>7.843333333333334</v>
+      </c>
     </row>
     <row r="127" ht="12.8" customHeight="1" s="6">
       <c r="A127" s="8" t="inlineStr">
@@ -3042,6 +3425,9 @@
           <t>1024</t>
         </is>
       </c>
+      <c r="E127" s="5" t="n">
+        <v>-2.846666666666666</v>
+      </c>
     </row>
     <row r="128" ht="12.8" customHeight="1" s="6">
       <c r="A128" s="8" t="inlineStr">
@@ -3062,6 +3448,9 @@
           <t>312</t>
         </is>
       </c>
+      <c r="E128" s="5" t="n">
+        <v>-19.04333333333333</v>
+      </c>
     </row>
     <row r="129" ht="12.8" customHeight="1" s="6">
       <c r="A129" s="8" t="inlineStr">
@@ -3082,6 +3471,9 @@
           <t>686</t>
         </is>
       </c>
+      <c r="E129" s="5" t="n">
+        <v>-0.7466666666666667</v>
+      </c>
     </row>
     <row r="130" ht="12.8" customHeight="1" s="6">
       <c r="A130" s="8" t="inlineStr">
@@ -3102,6 +3494,9 @@
           <t>3835</t>
         </is>
       </c>
+      <c r="E130" s="5" t="n">
+        <v>-8.68</v>
+      </c>
     </row>
     <row r="131" ht="12.8" customHeight="1" s="6">
       <c r="A131" s="8" t="inlineStr">
@@ -3122,6 +3517,9 @@
           <t>1234</t>
         </is>
       </c>
+      <c r="E131" s="5" t="n">
+        <v>4.486666666666667</v>
+      </c>
     </row>
     <row r="132" ht="12.8" customHeight="1" s="6">
       <c r="A132" s="8" t="inlineStr">
@@ -3142,6 +3540,9 @@
           <t>1801</t>
         </is>
       </c>
+      <c r="E132" s="5" t="n">
+        <v>2.163333333333334</v>
+      </c>
     </row>
     <row r="133" ht="12.8" customHeight="1" s="6">
       <c r="A133" s="8" t="inlineStr">
@@ -3162,6 +3563,9 @@
           <t>3106</t>
         </is>
       </c>
+      <c r="E133" s="5" t="n">
+        <v>2.266666666666667</v>
+      </c>
     </row>
     <row r="134" ht="12.8" customHeight="1" s="6">
       <c r="A134" s="8" t="inlineStr">
@@ -3182,6 +3586,9 @@
           <t>1046</t>
         </is>
       </c>
+      <c r="E134" s="5" t="n">
+        <v>1.206666666666667</v>
+      </c>
     </row>
     <row r="135" ht="12.8" customHeight="1" s="6">
       <c r="A135" s="8" t="inlineStr">
@@ -3202,6 +3609,9 @@
           <t>1174</t>
         </is>
       </c>
+      <c r="E135" s="5" t="n">
+        <v>4.523333333333333</v>
+      </c>
     </row>
     <row r="136" ht="12.8" customHeight="1" s="6">
       <c r="A136" s="8" t="inlineStr">
@@ -3222,6 +3632,9 @@
           <t>6528</t>
         </is>
       </c>
+      <c r="E136" s="5" t="n">
+        <v>9.466666666666667</v>
+      </c>
     </row>
     <row r="137" ht="12.8" customHeight="1" s="6">
       <c r="A137" s="8" t="inlineStr">
@@ -3242,6 +3655,9 @@
           <t>50818</t>
         </is>
       </c>
+      <c r="E137" s="5" t="n">
+        <v>15.92</v>
+      </c>
     </row>
     <row r="138" ht="12.8" customHeight="1" s="6">
       <c r="A138" s="8" t="inlineStr">
@@ -3262,6 +3678,9 @@
           <t>3432</t>
         </is>
       </c>
+      <c r="E138" s="5" t="n">
+        <v>-2.083333333333333</v>
+      </c>
     </row>
     <row r="139" ht="12.8" customHeight="1" s="6">
       <c r="A139" s="8" t="inlineStr">
@@ -3282,6 +3701,9 @@
           <t>305</t>
         </is>
       </c>
+      <c r="E139" s="5" t="n">
+        <v>-13.93</v>
+      </c>
     </row>
     <row r="140" ht="12.8" customHeight="1" s="6">
       <c r="A140" s="8" t="inlineStr">
@@ -3302,6 +3724,9 @@
           <t>11730</t>
         </is>
       </c>
+      <c r="E140" s="5" t="n">
+        <v>-2.026666666666667</v>
+      </c>
     </row>
     <row r="141" ht="12.8" customHeight="1" s="6">
       <c r="A141" s="8" t="inlineStr">
@@ -3322,6 +3747,9 @@
           <t>2502</t>
         </is>
       </c>
+      <c r="E141" s="5" t="n">
+        <v>1.146666666666667</v>
+      </c>
     </row>
     <row r="142" ht="12.8" customHeight="1" s="6">
       <c r="A142" s="8" t="inlineStr">
@@ -3342,6 +3770,9 @@
           <t>349104</t>
         </is>
       </c>
+      <c r="E142" s="5" t="n">
+        <v>4.896666666666667</v>
+      </c>
     </row>
     <row r="143" ht="12.8" customHeight="1" s="6">
       <c r="A143" s="8" t="inlineStr">
@@ -3362,6 +3793,9 @@
           <t>988</t>
         </is>
       </c>
+      <c r="E143" s="5" t="n">
+        <v>-1.106666666666667</v>
+      </c>
     </row>
     <row r="144" ht="12.8" customHeight="1" s="6">
       <c r="A144" s="8" t="inlineStr">
@@ -3382,6 +3816,9 @@
           <t>2295</t>
         </is>
       </c>
+      <c r="E144" s="5" t="n">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="145" ht="12.8" customHeight="1" s="6">
       <c r="A145" s="8" t="inlineStr">
@@ -3402,6 +3839,9 @@
           <t>877</t>
         </is>
       </c>
+      <c r="E145" s="5" t="n">
+        <v>9.383333333333333</v>
+      </c>
     </row>
     <row r="146" ht="12.8" customHeight="1" s="6">
       <c r="A146" s="8" t="inlineStr">
@@ -3422,6 +3862,9 @@
           <t>2359</t>
         </is>
       </c>
+      <c r="E146" s="5" t="n">
+        <v>6.533333333333334</v>
+      </c>
     </row>
     <row r="147" ht="12.8" customHeight="1" s="6">
       <c r="A147" s="8" t="inlineStr">
@@ -3442,6 +3885,9 @@
           <t>1187</t>
         </is>
       </c>
+      <c r="E147" s="5" t="n">
+        <v>2.093333333333333</v>
+      </c>
     </row>
     <row r="148" ht="12.8" customHeight="1" s="6">
       <c r="A148" s="8" t="inlineStr">
@@ -3462,6 +3908,9 @@
           <t>8130</t>
         </is>
       </c>
+      <c r="E148" s="5" t="n">
+        <v>-2.33</v>
+      </c>
     </row>
     <row r="149" ht="12.8" customHeight="1" s="6">
       <c r="A149" s="8" t="inlineStr">
@@ -3482,6 +3931,9 @@
           <t>4674</t>
         </is>
       </c>
+      <c r="E149" s="5" t="n">
+        <v>1.57</v>
+      </c>
     </row>
     <row r="150" ht="12.8" customHeight="1" s="6">
       <c r="A150" s="8" t="inlineStr">
@@ -3502,6 +3954,9 @@
           <t>10984</t>
         </is>
       </c>
+      <c r="E150" s="5" t="n">
+        <v>0.8933333333333334</v>
+      </c>
     </row>
     <row r="151" ht="12.8" customHeight="1" s="6">
       <c r="A151" s="8" t="inlineStr">
@@ -3522,6 +3977,9 @@
           <t>15957</t>
         </is>
       </c>
+      <c r="E151" s="5" t="n">
+        <v>0.1033333333333333</v>
+      </c>
     </row>
     <row r="152" ht="12.8" customHeight="1" s="6">
       <c r="A152" s="8" t="inlineStr">
@@ -3542,6 +4000,9 @@
           <t>57914</t>
         </is>
       </c>
+      <c r="E152" s="5" t="n">
+        <v>1.43</v>
+      </c>
     </row>
     <row r="153" ht="12.8" customHeight="1" s="6">
       <c r="A153" s="8" t="inlineStr">
@@ -3562,6 +4023,9 @@
           <t>3450</t>
         </is>
       </c>
+      <c r="E153" s="5" t="n">
+        <v>1.42</v>
+      </c>
     </row>
     <row r="154" ht="12.8" customHeight="1" s="6">
       <c r="A154" s="8" t="inlineStr">
@@ -3582,6 +4046,9 @@
           <t>3681</t>
         </is>
       </c>
+      <c r="E154" s="5" t="n">
+        <v>0.1433333333333333</v>
+      </c>
     </row>
     <row r="155" ht="12.8" customHeight="1" s="6">
       <c r="A155" s="8" t="inlineStr">
@@ -3602,6 +4069,9 @@
           <t>12748</t>
         </is>
       </c>
+      <c r="E155" s="5" t="n">
+        <v>3.433333333333334</v>
+      </c>
     </row>
     <row r="156" ht="12.8" customHeight="1" s="6">
       <c r="A156" s="8" t="inlineStr">
@@ -3622,6 +4092,9 @@
           <t>10254</t>
         </is>
       </c>
+      <c r="E156" s="5" t="n">
+        <v>1.893333333333333</v>
+      </c>
     </row>
     <row r="157" ht="12.8" customHeight="1" s="6">
       <c r="A157" s="8" t="inlineStr">
@@ -3642,6 +4115,9 @@
           <t>21846</t>
         </is>
       </c>
+      <c r="E157" s="5" t="n">
+        <v>1.576666666666667</v>
+      </c>
     </row>
     <row r="158" ht="12.8" customHeight="1" s="6">
       <c r="A158" s="8" t="inlineStr">
@@ -3662,6 +4138,9 @@
           <t>10373</t>
         </is>
       </c>
+      <c r="E158" s="5" t="n">
+        <v>1.626666666666667</v>
+      </c>
     </row>
     <row r="159" ht="12.8" customHeight="1" s="6">
       <c r="A159" s="8" t="inlineStr">
@@ -3682,6 +4161,9 @@
           <t>1222</t>
         </is>
       </c>
+      <c r="E159" s="5" t="n">
+        <v>-0.6733333333333333</v>
+      </c>
     </row>
     <row r="160" ht="12.8" customHeight="1" s="6">
       <c r="A160" s="8" t="inlineStr">
@@ -3702,6 +4184,9 @@
           <t>6497</t>
         </is>
       </c>
+      <c r="E160" s="5" t="n">
+        <v>8.779999999999999</v>
+      </c>
     </row>
     <row r="161" ht="12.8" customHeight="1" s="6">
       <c r="A161" s="8" t="inlineStr">
@@ -3722,6 +4207,9 @@
           <t>19764</t>
         </is>
       </c>
+      <c r="E161" s="5" t="n">
+        <v>7.036666666666666</v>
+      </c>
     </row>
     <row r="162" ht="12.8" customHeight="1" s="6">
       <c r="A162" s="8" t="inlineStr">
@@ -3742,6 +4230,9 @@
           <t>416</t>
         </is>
       </c>
+      <c r="E162" s="5" t="n">
+        <v>-16.35</v>
+      </c>
     </row>
     <row r="163" ht="12.8" customHeight="1" s="6">
       <c r="A163" s="8" t="inlineStr">
@@ -3762,6 +4253,9 @@
           <t>5062</t>
         </is>
       </c>
+      <c r="E163" s="5" t="n">
+        <v>-2.74</v>
+      </c>
     </row>
     <row r="164" ht="12.8" customHeight="1" s="6">
       <c r="A164" s="8" t="inlineStr">
@@ -3782,6 +4276,9 @@
           <t>2540</t>
         </is>
       </c>
+      <c r="E164" s="5" t="n">
+        <v>-0.7533333333333333</v>
+      </c>
     </row>
     <row r="165" ht="12.8" customHeight="1" s="6">
       <c r="A165" s="8" t="inlineStr">
@@ -3802,6 +4299,9 @@
           <t>5959</t>
         </is>
       </c>
+      <c r="E165" s="5" t="n">
+        <v>-0.13</v>
+      </c>
     </row>
     <row r="166" ht="12.8" customHeight="1" s="6">
       <c r="A166" s="8" t="inlineStr">
@@ -3822,6 +4322,9 @@
           <t>6819</t>
         </is>
       </c>
+      <c r="E166" s="5" t="n">
+        <v>3.183333333333334</v>
+      </c>
     </row>
     <row r="167" ht="12.8" customHeight="1" s="6">
       <c r="A167" s="8" t="inlineStr">
@@ -3842,6 +4345,9 @@
           <t>3514</t>
         </is>
       </c>
+      <c r="E167" s="5" t="n">
+        <v>3.353333333333333</v>
+      </c>
     </row>
     <row r="168" ht="12.8" customHeight="1" s="6">
       <c r="A168" s="8" t="inlineStr">
@@ -3862,6 +4368,9 @@
           <t>1674</t>
         </is>
       </c>
+      <c r="E168" s="5" t="n">
+        <v>1.71</v>
+      </c>
     </row>
     <row r="169" ht="12.8" customHeight="1" s="6">
       <c r="A169" s="8" t="inlineStr">
@@ -3882,6 +4391,9 @@
           <t>1580</t>
         </is>
       </c>
+      <c r="E169" s="5" t="n">
+        <v>0.2333333333333333</v>
+      </c>
     </row>
     <row r="170" ht="12.8" customHeight="1" s="6">
       <c r="A170" s="8" t="inlineStr">
@@ -3902,6 +4414,9 @@
           <t>758</t>
         </is>
       </c>
+      <c r="E170" s="5" t="n">
+        <v>0.1233333333333333</v>
+      </c>
     </row>
     <row r="171" ht="12.8" customHeight="1" s="6">
       <c r="A171" s="8" t="inlineStr">
@@ -3922,6 +4437,9 @@
           <t>12269</t>
         </is>
       </c>
+      <c r="E171" s="5" t="n">
+        <v>4.16</v>
+      </c>
     </row>
     <row r="172" ht="12.8" customHeight="1" s="6">
       <c r="A172" s="8" t="inlineStr">
@@ -3942,6 +4460,9 @@
           <t>7074</t>
         </is>
       </c>
+      <c r="E172" s="5" t="n">
+        <v>2.64</v>
+      </c>
     </row>
     <row r="173" ht="12.8" customHeight="1" s="6">
       <c r="A173" s="8" t="inlineStr">
@@ -3962,6 +4483,9 @@
           <t>4581</t>
         </is>
       </c>
+      <c r="E173" s="5" t="n">
+        <v>-4.223333333333334</v>
+      </c>
     </row>
     <row r="174" ht="12.8" customHeight="1" s="6">
       <c r="A174" s="8" t="inlineStr">
@@ -3982,6 +4506,9 @@
           <t>3173</t>
         </is>
       </c>
+      <c r="E174" s="5" t="n">
+        <v>1.256666666666667</v>
+      </c>
     </row>
     <row r="175" ht="12.8" customHeight="1" s="6">
       <c r="A175" s="8" t="inlineStr">
@@ -4002,6 +4529,9 @@
           <t>4707</t>
         </is>
       </c>
+      <c r="E175" s="5" t="n">
+        <v>1.203333333333333</v>
+      </c>
     </row>
     <row r="176" ht="12.8" customHeight="1" s="6">
       <c r="A176" s="8" t="inlineStr">
@@ -4022,6 +4552,9 @@
           <t>26217</t>
         </is>
       </c>
+      <c r="E176" s="5" t="n">
+        <v>8.803333333333333</v>
+      </c>
     </row>
     <row r="177" ht="12.8" customHeight="1" s="6">
       <c r="A177" s="8" t="inlineStr">
@@ -4042,6 +4575,9 @@
           <t>996</t>
         </is>
       </c>
+      <c r="E177" s="5" t="n">
+        <v>5.796666666666667</v>
+      </c>
     </row>
     <row r="178" ht="12.8" customHeight="1" s="6">
       <c r="A178" s="8" t="inlineStr">
@@ -4062,6 +4598,9 @@
           <t>1672</t>
         </is>
       </c>
+      <c r="E178" s="5" t="n">
+        <v>2.086666666666666</v>
+      </c>
     </row>
     <row r="179" ht="12.8" customHeight="1" s="6">
       <c r="A179" s="8" t="inlineStr">
@@ -4082,6 +4621,9 @@
           <t>32119</t>
         </is>
       </c>
+      <c r="E179" s="5" t="n">
+        <v>5.489999999999999</v>
+      </c>
     </row>
     <row r="180" ht="12.8" customHeight="1" s="6">
       <c r="A180" s="8" t="inlineStr">
@@ -4102,6 +4644,9 @@
           <t>350</t>
         </is>
       </c>
+      <c r="E180" s="5" t="n">
+        <v>-0.04</v>
+      </c>
     </row>
     <row r="181" ht="12.8" customHeight="1" s="6">
       <c r="A181" s="8" t="inlineStr">
@@ -4122,6 +4667,9 @@
           <t>22176</t>
         </is>
       </c>
+      <c r="E181" s="5" t="n">
+        <v>-18.62</v>
+      </c>
     </row>
     <row r="182" ht="12.8" customHeight="1" s="6">
       <c r="A182" s="8" t="inlineStr">
@@ -4142,6 +4690,9 @@
           <t>7306</t>
         </is>
       </c>
+      <c r="E182" s="5" t="n">
+        <v>3.71</v>
+      </c>
     </row>
     <row r="183" ht="12.8" customHeight="1" s="6">
       <c r="A183" s="8" t="inlineStr">
@@ -4162,6 +4713,9 @@
           <t>5736</t>
         </is>
       </c>
+      <c r="E183" s="5" t="n">
+        <v>1.463333333333333</v>
+      </c>
     </row>
     <row r="184" ht="12.8" customHeight="1" s="6">
       <c r="A184" s="8" t="inlineStr">
@@ -4182,6 +4736,9 @@
           <t>4626</t>
         </is>
       </c>
+      <c r="E184" s="5" t="n">
+        <v>-0.4966666666666666</v>
+      </c>
     </row>
     <row r="185" ht="12.8" customHeight="1" s="6">
       <c r="A185" s="8" t="inlineStr">
@@ -4202,6 +4759,9 @@
           <t>876</t>
         </is>
       </c>
+      <c r="E185" s="5" t="n">
+        <v>0.5033333333333333</v>
+      </c>
     </row>
     <row r="186" ht="12.8" customHeight="1" s="6">
       <c r="A186" s="8" t="inlineStr">
@@ -4222,6 +4782,9 @@
           <t>2193</t>
         </is>
       </c>
+      <c r="E186" s="5" t="n">
+        <v>1.076666666666667</v>
+      </c>
     </row>
     <row r="187" ht="12.8" customHeight="1" s="6">
       <c r="A187" s="8" t="inlineStr">
@@ -4242,6 +4805,9 @@
           <t>710</t>
         </is>
       </c>
+      <c r="E187" s="5" t="n">
+        <v>-3.176666666666666</v>
+      </c>
     </row>
     <row r="188" ht="12.8" customHeight="1" s="6">
       <c r="A188" s="8" t="inlineStr">
@@ -4262,6 +4828,9 @@
           <t>946</t>
         </is>
       </c>
+      <c r="E188" s="5" t="n">
+        <v>-4.803333333333334</v>
+      </c>
     </row>
     <row r="189" ht="12.8" customHeight="1" s="6">
       <c r="A189" s="8" t="inlineStr">
@@ -4282,6 +4851,9 @@
           <t>1037</t>
         </is>
       </c>
+      <c r="E189" s="5" t="n">
+        <v>-0.7233333333333333</v>
+      </c>
     </row>
     <row r="190" ht="12.8" customHeight="1" s="6">
       <c r="A190" s="8" t="inlineStr">
@@ -4302,6 +4874,9 @@
           <t>2134</t>
         </is>
       </c>
+      <c r="E190" s="5" t="n">
+        <v>4.43</v>
+      </c>
     </row>
     <row r="191" ht="12.8" customHeight="1" s="6">
       <c r="A191" s="8" t="inlineStr">
@@ -4322,6 +4897,9 @@
           <t>2432</t>
         </is>
       </c>
+      <c r="E191" s="5" t="n">
+        <v>4.003333333333333</v>
+      </c>
     </row>
     <row r="192" ht="12.8" customHeight="1" s="6">
       <c r="A192" s="8" t="inlineStr">
@@ -4342,6 +4920,9 @@
           <t>1395</t>
         </is>
       </c>
+      <c r="E192" s="5" t="n">
+        <v>0.3766666666666666</v>
+      </c>
     </row>
     <row r="193" ht="12.8" customHeight="1" s="6">
       <c r="A193" s="8" t="inlineStr">
@@ -4362,6 +4943,9 @@
           <t>20291</t>
         </is>
       </c>
+      <c r="E193" s="5" t="n">
+        <v>2.546666666666666</v>
+      </c>
     </row>
     <row r="194" ht="12.8" customHeight="1" s="6">
       <c r="A194" s="8" t="inlineStr">
@@ -4382,6 +4966,9 @@
           <t>3733</t>
         </is>
       </c>
+      <c r="E194" s="5" t="n">
+        <v>2.593333333333333</v>
+      </c>
     </row>
     <row r="195" ht="12.8" customHeight="1" s="6">
       <c r="A195" s="8" t="inlineStr">
@@ -4402,6 +4989,9 @@
           <t>6497</t>
         </is>
       </c>
+      <c r="E195" s="5" t="n">
+        <v>8.25</v>
+      </c>
     </row>
     <row r="196" ht="12.8" customHeight="1" s="6">
       <c r="A196" s="8" t="inlineStr">
@@ -4422,6 +5012,9 @@
           <t>5110</t>
         </is>
       </c>
+      <c r="E196" s="5" t="n">
+        <v>1.36</v>
+      </c>
     </row>
     <row r="197" ht="12.8" customHeight="1" s="6">
       <c r="A197" s="8" t="inlineStr">
@@ -4442,6 +5035,9 @@
           <t>8795</t>
         </is>
       </c>
+      <c r="E197" s="5" t="n">
+        <v>3.51</v>
+      </c>
     </row>
     <row r="198" ht="12.8" customHeight="1" s="6">
       <c r="A198" s="8" t="inlineStr">
@@ -4462,6 +5058,9 @@
           <t>67539</t>
         </is>
       </c>
+      <c r="E198" s="5" t="n">
+        <v>3.866666666666667</v>
+      </c>
     </row>
     <row r="199" ht="12.8" customHeight="1" s="6">
       <c r="A199" s="8" t="inlineStr">
@@ -4482,6 +5081,9 @@
           <t>12866</t>
         </is>
       </c>
+      <c r="E199" s="5" t="n">
+        <v>7.97</v>
+      </c>
     </row>
     <row r="200" ht="12.8" customHeight="1" s="6">
       <c r="A200" s="8" t="inlineStr">
@@ -4502,6 +5104,9 @@
           <t>7420</t>
         </is>
       </c>
+      <c r="E200" s="5" t="n">
+        <v>1.203333333333333</v>
+      </c>
     </row>
     <row r="201" ht="12.8" customHeight="1" s="6">
       <c r="A201" s="8" t="inlineStr">
@@ -4522,6 +5127,9 @@
           <t>2210</t>
         </is>
       </c>
+      <c r="E201" s="5" t="n">
+        <v>3.02</v>
+      </c>
     </row>
     <row r="202" ht="12.8" customHeight="1" s="6">
       <c r="A202" s="8" t="inlineStr">
@@ -4542,6 +5150,9 @@
           <t>690</t>
         </is>
       </c>
+      <c r="E202" s="5" t="n">
+        <v>-2.103333333333333</v>
+      </c>
     </row>
     <row r="203" ht="12.8" customHeight="1" s="6">
       <c r="A203" s="8" t="inlineStr">
@@ -4562,6 +5173,9 @@
           <t>8427</t>
         </is>
       </c>
+      <c r="E203" s="5" t="n">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="204" ht="12.8" customHeight="1" s="6">
       <c r="A204" s="8" t="inlineStr">
@@ -4582,6 +5196,9 @@
           <t>4945</t>
         </is>
       </c>
+      <c r="E204" s="5" t="n">
+        <v>4.033333333333333</v>
+      </c>
     </row>
     <row r="205" ht="12.8" customHeight="1" s="6">
       <c r="A205" s="8" t="inlineStr">
@@ -4602,6 +5219,9 @@
           <t>850</t>
         </is>
       </c>
+      <c r="E205" s="5" t="n">
+        <v>2.61</v>
+      </c>
     </row>
     <row r="206" ht="12.8" customHeight="1" s="6">
       <c r="A206" s="8" t="inlineStr">
@@ -4622,6 +5242,9 @@
           <t>555</t>
         </is>
       </c>
+      <c r="E206" s="5" t="n">
+        <v>4.126666666666667</v>
+      </c>
     </row>
     <row r="207" ht="12.8" customHeight="1" s="6">
       <c r="A207" s="8" t="inlineStr">
@@ -4642,6 +5265,9 @@
           <t>2918</t>
         </is>
       </c>
+      <c r="E207" s="5" t="n">
+        <v>7.096666666666667</v>
+      </c>
     </row>
     <row r="208" ht="12.8" customHeight="1" s="6">
       <c r="A208" s="8" t="inlineStr">
@@ -4662,6 +5288,9 @@
           <t>2656</t>
         </is>
       </c>
+      <c r="E208" s="5" t="n">
+        <v>1.916666666666667</v>
+      </c>
     </row>
     <row r="209" ht="12.8" customHeight="1" s="6">
       <c r="A209" s="8" t="inlineStr">
@@ -4682,6 +5311,9 @@
           <t>26697</t>
         </is>
       </c>
+      <c r="E209" s="5" t="n">
+        <v>7.803333333333334</v>
+      </c>
     </row>
     <row r="210" ht="12.8" customHeight="1" s="6">
       <c r="A210" s="8" t="inlineStr">
@@ -4702,6 +5334,9 @@
           <t>1293</t>
         </is>
       </c>
+      <c r="E210" s="5" t="n">
+        <v>-0.2166666666666667</v>
+      </c>
     </row>
     <row r="211" ht="12.8" customHeight="1" s="6">
       <c r="A211" s="8" t="inlineStr">
@@ -4722,6 +5357,9 @@
           <t>1466</t>
         </is>
       </c>
+      <c r="E211" s="5" t="n">
+        <v>1.62</v>
+      </c>
     </row>
     <row r="212" ht="12.8" customHeight="1" s="6">
       <c r="A212" s="8" t="inlineStr">
@@ -4742,6 +5380,9 @@
           <t>5600</t>
         </is>
       </c>
+      <c r="E212" s="5" t="n">
+        <v>7.656666666666666</v>
+      </c>
     </row>
     <row r="213" ht="12.8" customHeight="1" s="6">
       <c r="A213" s="8" t="inlineStr">
@@ -4762,6 +5403,9 @@
           <t>14338</t>
         </is>
       </c>
+      <c r="E213" s="5" t="n">
+        <v>2.683333333333334</v>
+      </c>
     </row>
     <row r="214" ht="12.8" customHeight="1" s="6">
       <c r="A214" s="8" t="inlineStr">
@@ -4782,6 +5426,9 @@
           <t>464</t>
         </is>
       </c>
+      <c r="E214" s="5" t="n">
+        <v>-2.836666666666666</v>
+      </c>
     </row>
     <row r="215" ht="12.8" customHeight="1" s="6">
       <c r="A215" s="8" t="inlineStr">
@@ -4802,6 +5449,9 @@
           <t>3468</t>
         </is>
       </c>
+      <c r="E215" s="5" t="n">
+        <v>1.916666666666667</v>
+      </c>
     </row>
     <row r="216" ht="12.8" customHeight="1" s="6">
       <c r="A216" s="8" t="inlineStr">
@@ -4822,6 +5472,9 @@
           <t>9652</t>
         </is>
       </c>
+      <c r="E216" s="5" t="n">
+        <v>2.166666666666667</v>
+      </c>
     </row>
     <row r="217" ht="12.8" customHeight="1" s="6">
       <c r="A217" s="8" t="inlineStr">
@@ -4842,6 +5495,9 @@
           <t>6564</t>
         </is>
       </c>
+      <c r="E217" s="5" t="n">
+        <v>0.6566666666666666</v>
+      </c>
     </row>
     <row r="218" ht="12.8" customHeight="1" s="6">
       <c r="A218" s="8" t="inlineStr">
@@ -4862,6 +5518,9 @@
           <t>2044</t>
         </is>
       </c>
+      <c r="E218" s="5" t="n">
+        <v>0.7833333333333333</v>
+      </c>
     </row>
     <row r="219" ht="12.8" customHeight="1" s="6">
       <c r="A219" s="8" t="inlineStr">
@@ -4882,6 +5541,9 @@
           <t>3705</t>
         </is>
       </c>
+      <c r="E219" s="5" t="n">
+        <v>1.496666666666667</v>
+      </c>
     </row>
     <row r="220" ht="12.8" customHeight="1" s="6">
       <c r="A220" s="8" t="inlineStr">
@@ -4902,6 +5564,9 @@
           <t>841</t>
         </is>
       </c>
+      <c r="E220" s="5" t="n">
+        <v>-8.359999999999999</v>
+      </c>
     </row>
     <row r="221" ht="12.8" customHeight="1" s="6">
       <c r="A221" s="8" t="inlineStr">
@@ -4922,6 +5587,9 @@
           <t>7980</t>
         </is>
       </c>
+      <c r="E221" s="5" t="n">
+        <v>0.68</v>
+      </c>
     </row>
     <row r="222" ht="12.8" customHeight="1" s="6">
       <c r="A222" s="8" t="inlineStr">
@@ -4942,6 +5610,9 @@
           <t>30439</t>
         </is>
       </c>
+      <c r="E222" s="5" t="n">
+        <v>3.006666666666666</v>
+      </c>
     </row>
     <row r="223" ht="12.8" customHeight="1" s="6">
       <c r="A223" s="8" t="inlineStr">
@@ -4962,6 +5633,9 @@
           <t>841</t>
         </is>
       </c>
+      <c r="E223" s="5" t="n">
+        <v>-1.466666666666667</v>
+      </c>
     </row>
     <row r="224" ht="12.8" customHeight="1" s="6">
       <c r="A224" s="8" t="inlineStr">
@@ -4982,6 +5656,9 @@
           <t>1107</t>
         </is>
       </c>
+      <c r="E224" s="5" t="n">
+        <v>2.423333333333333</v>
+      </c>
     </row>
     <row r="225" ht="12.8" customHeight="1" s="6">
       <c r="A225" s="8" t="inlineStr">
@@ -5002,6 +5679,9 @@
           <t>7988</t>
         </is>
       </c>
+      <c r="E225" s="5" t="n">
+        <v>2.996666666666667</v>
+      </c>
     </row>
     <row r="226" ht="12.8" customHeight="1" s="6">
       <c r="A226" s="8" t="inlineStr">
@@ -5022,6 +5702,9 @@
           <t>614</t>
         </is>
       </c>
+      <c r="E226" s="5" t="n">
+        <v>16.17</v>
+      </c>
     </row>
     <row r="227" ht="12.8" customHeight="1" s="6">
       <c r="A227" s="8" t="inlineStr">
@@ -5042,6 +5725,9 @@
           <t>14370</t>
         </is>
       </c>
+      <c r="E227" s="5" t="n">
+        <v>4.196666666666666</v>
+      </c>
     </row>
     <row r="228" ht="12.8" customHeight="1" s="6">
       <c r="A228" s="8" t="inlineStr">
@@ -5062,6 +5748,9 @@
           <t>568</t>
         </is>
       </c>
+      <c r="E228" s="5" t="n">
+        <v>4.75</v>
+      </c>
     </row>
     <row r="229" ht="12.8" customHeight="1" s="6">
       <c r="A229" s="8" t="inlineStr">
@@ -5082,6 +5771,9 @@
           <t>6630</t>
         </is>
       </c>
+      <c r="E229" s="5" t="n">
+        <v>2.316666666666667</v>
+      </c>
     </row>
     <row r="230" ht="12.8" customHeight="1" s="6">
       <c r="A230" s="8" t="inlineStr">
@@ -5102,6 +5794,9 @@
           <t>2035</t>
         </is>
       </c>
+      <c r="E230" s="5" t="n">
+        <v>1.003333333333333</v>
+      </c>
     </row>
     <row r="231" ht="12.8" customHeight="1" s="6">
       <c r="A231" s="8" t="inlineStr">
@@ -5122,6 +5817,9 @@
           <t>4020</t>
         </is>
       </c>
+      <c r="E231" s="5" t="n">
+        <v>3.826666666666667</v>
+      </c>
     </row>
     <row r="232" ht="12.8" customHeight="1" s="6">
       <c r="A232" s="8" t="inlineStr">
@@ -5142,6 +5840,9 @@
           <t>1535</t>
         </is>
       </c>
+      <c r="E232" s="5" t="n">
+        <v>1.94</v>
+      </c>
     </row>
     <row r="233" ht="12.8" customHeight="1" s="6">
       <c r="A233" s="8" t="inlineStr">
@@ -5162,6 +5863,9 @@
           <t>3469</t>
         </is>
       </c>
+      <c r="E233" s="5" t="n">
+        <v>1.756666666666667</v>
+      </c>
     </row>
     <row r="234" ht="12.8" customHeight="1" s="6">
       <c r="A234" s="8" t="inlineStr">
@@ -5182,6 +5886,9 @@
           <t>43213</t>
         </is>
       </c>
+      <c r="E234" s="5" t="n">
+        <v>3.063333333333333</v>
+      </c>
     </row>
     <row r="235" ht="12.8" customHeight="1" s="6">
       <c r="A235" s="8" t="inlineStr">
@@ -5202,6 +5909,9 @@
           <t>21651</t>
         </is>
       </c>
+      <c r="E235" s="5" t="n">
+        <v>3.693333333333333</v>
+      </c>
     </row>
     <row r="236" ht="12.8" customHeight="1" s="6">
       <c r="A236" s="8" t="inlineStr">
@@ -5222,6 +5932,9 @@
           <t>60914</t>
         </is>
       </c>
+      <c r="E236" s="5" t="n">
+        <v>3.556666666666667</v>
+      </c>
     </row>
     <row r="237" ht="12.8" customHeight="1" s="6">
       <c r="A237" s="8" t="inlineStr">
@@ -5242,6 +5955,9 @@
           <t>5182</t>
         </is>
       </c>
+      <c r="E237" s="5" t="n">
+        <v>0.5633333333333334</v>
+      </c>
     </row>
     <row r="238" ht="12.8" customHeight="1" s="6">
       <c r="A238" s="8" t="inlineStr">
@@ -5262,6 +5978,9 @@
           <t>1938</t>
         </is>
       </c>
+      <c r="E238" s="5" t="n">
+        <v>2.853333333333333</v>
+      </c>
     </row>
     <row r="239" ht="12.8" customHeight="1" s="6">
       <c r="A239" s="8" t="inlineStr">
@@ -5282,6 +6001,9 @@
           <t>3413</t>
         </is>
       </c>
+      <c r="E239" s="5" t="n">
+        <v>7.656666666666666</v>
+      </c>
     </row>
     <row r="240" ht="12.8" customHeight="1" s="6">
       <c r="A240" s="8" t="inlineStr">
@@ -5302,6 +6024,9 @@
           <t>2355</t>
         </is>
       </c>
+      <c r="E240" s="5" t="n">
+        <v>7.97</v>
+      </c>
     </row>
     <row r="241" ht="12.8" customHeight="1" s="6">
       <c r="A241" s="8" t="inlineStr">
@@ -5322,6 +6047,9 @@
           <t>1433</t>
         </is>
       </c>
+      <c r="E241" s="5" t="n">
+        <v>3.74</v>
+      </c>
     </row>
     <row r="242" ht="12.8" customHeight="1" s="6">
       <c r="A242" s="8" t="inlineStr">
@@ -5342,6 +6070,9 @@
           <t>930</t>
         </is>
       </c>
+      <c r="E242" s="5" t="n">
+        <v>15.01</v>
+      </c>
     </row>
     <row r="243" ht="12.8" customHeight="1" s="6">
       <c r="A243" s="8" t="inlineStr">
@@ -5362,6 +6093,9 @@
           <t>3646</t>
         </is>
       </c>
+      <c r="E243" s="5" t="n">
+        <v>-0.3766666666666666</v>
+      </c>
     </row>
     <row r="244" ht="12.8" customHeight="1" s="6">
       <c r="A244" s="8" t="inlineStr">
@@ -5382,6 +6116,9 @@
           <t>3116</t>
         </is>
       </c>
+      <c r="E244" s="5" t="n">
+        <v>0.8466666666666667</v>
+      </c>
     </row>
     <row r="245" ht="12.8" customHeight="1" s="6">
       <c r="A245" s="8" t="inlineStr">
@@ -5402,6 +6139,9 @@
           <t>7111</t>
         </is>
       </c>
+      <c r="E245" s="5" t="n">
+        <v>4.03</v>
+      </c>
     </row>
     <row r="246" ht="12.8" customHeight="1" s="6">
       <c r="A246" s="8" t="inlineStr">
@@ -5422,6 +6162,9 @@
           <t>3445</t>
         </is>
       </c>
+      <c r="E246" s="5" t="n">
+        <v>-0.6866666666666666</v>
+      </c>
     </row>
     <row r="247" ht="12.8" customHeight="1" s="6">
       <c r="A247" s="8" t="inlineStr">
@@ -5442,6 +6185,9 @@
           <t>2260</t>
         </is>
       </c>
+      <c r="E247" s="5" t="n">
+        <v>4.99</v>
+      </c>
     </row>
     <row r="248" ht="12.8" customHeight="1" s="6">
       <c r="A248" s="8" t="inlineStr">
@@ -5462,6 +6208,9 @@
           <t>6938</t>
         </is>
       </c>
+      <c r="E248" s="5" t="n">
+        <v>0.7933333333333333</v>
+      </c>
     </row>
     <row r="249" ht="12.8" customHeight="1" s="6">
       <c r="A249" s="8" t="inlineStr">
@@ -5482,6 +6231,9 @@
           <t>562</t>
         </is>
       </c>
+      <c r="E249" s="5" t="n">
+        <v>-46.80666666666666</v>
+      </c>
     </row>
     <row r="250" ht="12.8" customHeight="1" s="6">
       <c r="A250" s="8" t="inlineStr">
@@ -5502,6 +6254,9 @@
           <t>12293</t>
         </is>
       </c>
+      <c r="E250" s="5" t="n">
+        <v>4.093333333333333</v>
+      </c>
     </row>
     <row r="251" ht="12.8" customHeight="1" s="6">
       <c r="A251" s="8" t="inlineStr">
@@ -5518,6 +6273,7 @@
         <v>242968884</v>
       </c>
       <c r="D251" s="5" t="n"/>
+      <c r="E251" s="5" t="n"/>
     </row>
     <row r="252" ht="12.8" customHeight="1" s="6">
       <c r="A252" s="8" t="inlineStr">
@@ -5538,6 +6294,9 @@
           <t>10020</t>
         </is>
       </c>
+      <c r="E252" s="5" t="n">
+        <v>4.100000000000001</v>
+      </c>
     </row>
     <row r="253" ht="12.8" customHeight="1" s="6">
       <c r="A253" s="8" t="inlineStr">
@@ -5558,6 +6317,9 @@
           <t>100835</t>
         </is>
       </c>
+      <c r="E253" s="5" t="n">
+        <v>-0.98</v>
+      </c>
     </row>
     <row r="254" ht="12.8" customHeight="1" s="6">
       <c r="A254" s="8" t="inlineStr">
@@ -5578,6 +6340,9 @@
           <t>21986</t>
         </is>
       </c>
+      <c r="E254" s="5" t="n">
+        <v>10.14333333333333</v>
+      </c>
     </row>
     <row r="255" ht="12.8" customHeight="1" s="6">
       <c r="A255" s="8" t="inlineStr">
@@ -5598,6 +6363,9 @@
           <t>4332</t>
         </is>
       </c>
+      <c r="E255" s="5" t="n">
+        <v>2.73</v>
+      </c>
     </row>
     <row r="256" ht="12.8" customHeight="1" s="6">
       <c r="A256" s="8" t="inlineStr">
@@ -5618,6 +6386,9 @@
           <t>12341</t>
         </is>
       </c>
+      <c r="E256" s="5" t="n">
+        <v>0.96</v>
+      </c>
     </row>
     <row r="257" ht="12.8" customHeight="1" s="6">
       <c r="A257" s="8" t="inlineStr">
@@ -5638,6 +6409,9 @@
           <t>69790</t>
         </is>
       </c>
+      <c r="E257" s="5" t="n">
+        <v>1.536666666666667</v>
+      </c>
     </row>
     <row r="258" ht="12.8" customHeight="1" s="6">
       <c r="A258" s="8" t="inlineStr">
@@ -5658,6 +6432,9 @@
           <t>14267</t>
         </is>
       </c>
+      <c r="E258" s="5" t="n">
+        <v>3.32</v>
+      </c>
     </row>
     <row r="259" ht="12.8" customHeight="1" s="6">
       <c r="A259" s="8" t="inlineStr">
@@ -5678,6 +6455,9 @@
           <t>144102</t>
         </is>
       </c>
+      <c r="E259" s="5" t="n">
+        <v>3.29</v>
+      </c>
     </row>
     <row r="260" ht="12.8" customHeight="1" s="6">
       <c r="A260" s="8" t="inlineStr">
@@ -5698,6 +6478,9 @@
           <t>18274</t>
         </is>
       </c>
+      <c r="E260" s="5" t="n">
+        <v>-1.02</v>
+      </c>
     </row>
     <row r="261" ht="12.8" customHeight="1" s="6">
       <c r="A261" s="8" t="inlineStr">
@@ -5718,6 +6501,9 @@
           <t>473</t>
         </is>
       </c>
+      <c r="E261" s="5" t="n">
+        <v>-27.97333333333333</v>
+      </c>
     </row>
     <row r="262" ht="12.8" customHeight="1" s="6">
       <c r="A262" s="8" t="inlineStr">
@@ -5738,6 +6524,7 @@
           <t>794</t>
         </is>
       </c>
+      <c r="E262" s="5" t="n"/>
     </row>
     <row r="263" ht="12.8" customHeight="1" s="6">
       <c r="A263" s="8" t="inlineStr">
@@ -5758,6 +6545,9 @@
           <t>2313</t>
         </is>
       </c>
+      <c r="E263" s="5" t="n">
+        <v>0.9133333333333334</v>
+      </c>
     </row>
     <row r="264" ht="12.8" customHeight="1" s="6">
       <c r="A264" s="8" t="inlineStr">
@@ -16969,7 +17759,7 @@
       <c r="C826" s="9" t="n">
         <v>240424899</v>
       </c>
-      <c r="D826" t="inlineStr">
+      <c r="D826" s="5" t="inlineStr">
         <is>
           <t>1029</t>
         </is>

</xml_diff>